<commit_message>
Removed unnecessary test data
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -1,87 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B59772-81D0-49F0-B9CD-AE3CCBEBCF9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
-  <si>
-    <t>Test Case Name</t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>TC1</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>abc@xyz.com</t>
-  </si>
-  <si>
-    <t>Test@123</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>subject</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>order_reference</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>Customer service</t>
-  </si>
-  <si>
-    <t>abc@123.com</t>
-  </si>
-  <si>
-    <t>Testmessage1</t>
-  </si>
-  <si>
-    <t>Testmessage2</t>
-  </si>
-  <si>
-    <t>abc@234.com</t>
-  </si>
-  <si>
-    <t>abc123</t>
-  </si>
-  <si>
-    <t>bcd234</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,38 +24,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -128,37 +41,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -166,6 +56,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -214,7 +107,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -247,9 +140,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -282,6 +192,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -457,123 +384,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="F2" r:id="rId5"/>
-    <hyperlink ref="F3" r:id="rId6"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>